<commit_message>
[NOTIFICATIONS] Add Notifications API's
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="232">
   <si>
     <t>de_DE</t>
   </si>
@@ -688,6 +688,33 @@
   </si>
   <si>
     <t>Hola {0}, Tu cuenta ha sido activada con éxito, ¡podríamos empezar a registrar tus certificados digitales!.</t>
+  </si>
+  <si>
+    <t>mail_new_course_registration_requested_body</t>
+  </si>
+  <si>
+    <t>{0}, Hemos recibido tú solicitud de registro del curso {1}, en breve completaremos el registro!</t>
+  </si>
+  <si>
+    <t>{0}, We have received your registration request for the course {1}, we will complete the registration shortly!</t>
+  </si>
+  <si>
+    <t>mail_certificate_course_disabled_body</t>
+  </si>
+  <si>
+    <t>mail_certificate_course_enabled_body</t>
+  </si>
+  <si>
+    <t>{0}, El curso {1} ha sido deshabilitado en TCS, deberás volver a habilitarlo para que nuevos certificados puedan ser emitidos.</t>
+  </si>
+  <si>
+    <t>{0}, El curso {1} ha sido habilitado en TCS, nuevos certificados podrán ser emitidos.</t>
+  </si>
+  <si>
+    <t>{0}, The course {1} has been disabled in TCS, you must re-enable it so that new certificates can be issued.</t>
+  </si>
+  <si>
+    <t>{0}, The course {1} has been enabled in TCS, new certificates may be issued.</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1947,6 +1974,39 @@
         <v>221</v>
       </c>
     </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>227</v>
+      </c>
+      <c r="B79" t="s">
+        <v>229</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[COURSES] Create endpoint to remove courses as a CA.
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="241">
   <si>
     <t>de_DE</t>
   </si>
@@ -715,6 +715,33 @@
   </si>
   <si>
     <t>{0}, The course {1} has been enabled in TCS, new certificates may be issued.</t>
+  </si>
+  <si>
+    <t>delete_certification_course_failed</t>
+  </si>
+  <si>
+    <t>mail_certificate_course_deleted_subject_title</t>
+  </si>
+  <si>
+    <t>mail_certificate_course_deleted_body</t>
+  </si>
+  <si>
+    <t>{0}, El curso {1} ha sido eliminado en TCS, dejará de estar disponible para nuevos usuarios.</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al borrar el curso.</t>
+  </si>
+  <si>
+    <t>An error occurred while deleting the course.</t>
+  </si>
+  <si>
+    <t>{0}, El curso {1} ha sido eliminado.</t>
+  </si>
+  <si>
+    <t>{0}, Course {1} has been removed.</t>
+  </si>
+  <si>
+    <t>{0}, The course {1} has been removed from TCS, it will no longer be available to new users.</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2007,6 +2034,39 @@
         <v>231</v>
       </c>
     </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" t="s">
+        <v>236</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>233</v>
+      </c>
+      <c r="B81" t="s">
+        <v>238</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update default translations file
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="247">
   <si>
     <t>de_DE</t>
   </si>
@@ -742,6 +742,24 @@
   </si>
   <si>
     <t>{0}, The course {1} has been removed from TCS, it will no longer be available to new users.</t>
+  </si>
+  <si>
+    <t>partial_certification_course_update_failed</t>
+  </si>
+  <si>
+    <t>partial_certification_authority_update_failed</t>
+  </si>
+  <si>
+    <t>An error occurred while updating course information</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al actualizar la información de la entidad certificadora.</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al actualizar la información del curso.</t>
+  </si>
+  <si>
+    <t>An error occurred while updating the certification authority information.</t>
   </si>
 </sst>
 </file>
@@ -796,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,6 +824,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1147,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2088,28 @@
         <v>240</v>
       </c>
     </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>241</v>
+      </c>
+      <c r="B83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>242</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[NOTIFICATIONS] Implement FCM gateway
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="278">
   <si>
     <t>de_DE</t>
   </si>
@@ -582,15 +582,9 @@
     <t>{0}, Tú solicitud de emisión del certificado {1} ha sido aceptada!</t>
   </si>
   <si>
-    <t>{0}, Tú solicitud de emisión de certificado {1} ha sido rechazada!</t>
-  </si>
-  <si>
     <t>{0}, Your request to issue the certificate {1} has been accepted!</t>
   </si>
   <si>
-    <t>{0}, Your request to issue a certificate {1} has been rejected!</t>
-  </si>
-  <si>
     <t>mail_ca_enabled_body</t>
   </si>
   <si>
@@ -760,6 +754,105 @@
   </si>
   <si>
     <t>An error occurred while updating the certification authority information.</t>
+  </si>
+  <si>
+    <t>notification_certificate_enabled_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_enabled_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_disabled_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_disabled_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_issued_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_issued_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_renewed_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_renewed_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_request_accepted_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_request_accepted_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_request_rejected_title</t>
+  </si>
+  <si>
+    <t>notification_certificate_request_rejected_body</t>
+  </si>
+  <si>
+    <t>{0}, Tú solicitud de emisión de certificado {1} ha sido rechazada</t>
+  </si>
+  <si>
+    <t>{0}, Your request to issue a certificate {1} has been rejected</t>
+  </si>
+  <si>
+    <t>notification_certificate_visibility_changed_title</t>
+  </si>
+  <si>
+    <t>notification_student_issue_certificate_requested_title</t>
+  </si>
+  <si>
+    <t>notification_student_issue_certificate_requested_body</t>
+  </si>
+  <si>
+    <t>notification_ca_issue_certificate_requested_title</t>
+  </si>
+  <si>
+    <t>notification_ca_issue_certificate_requested_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_changed_to_visible_body</t>
+  </si>
+  <si>
+    <t>notification_certificate_changed_to_invisible_body</t>
+  </si>
+  <si>
+    <t>{0}, tú solicitud de emisión de certificado ha sido registrada!</t>
+  </si>
+  <si>
+    <t>{0}, your certificate issuance request has been registered!</t>
+  </si>
+  <si>
+    <t>{0}, hay una nueva solicitud de emisión de certificado</t>
+  </si>
+  <si>
+    <t>{0}, there is a new certificate issuance request.</t>
+  </si>
+  <si>
+    <t>{0}, En breve recibirás información sobre el progreso de tú solicitud de emisión de certificado.</t>
+  </si>
+  <si>
+    <t>{0}, You will shortly receive information on the progress of your certificate issuance request</t>
+  </si>
+  <si>
+    <t>{0}, revisa la solicitud de emisión de certificado para completar el proceso.</t>
+  </si>
+  <si>
+    <t>{0}, review the certificate issuance request to complete the process.</t>
+  </si>
+  <si>
+    <t>{0}, tú certificado {1} ha sido registrado con éxito!</t>
+  </si>
+  <si>
+    <t>{0}, your certificate {1} has been successfully registered!</t>
+  </si>
+  <si>
+    <t>{0}, podrás utilizar tú certificado proporcionando su identificador de emisión {1}</t>
+  </si>
+  <si>
+    <t>{0}, you can use your certificate by providing its issue identifier {1}</t>
   </si>
 </sst>
 </file>
@@ -1168,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1914,7 @@
         <v>186</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,10 +1922,10 @@
         <v>142</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>187</v>
+        <v>257</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>189</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1903,211 +1996,420 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="C66" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>197</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C70" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="C75" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="C76" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>221</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>225</v>
+      </c>
+      <c r="B79" t="s">
         <v>227</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B81" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="B83" t="s">
-        <v>245</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="C84" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C84" s="4" t="s">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>245</v>
+      </c>
+      <c r="B85" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>246</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>247</v>
+      </c>
+      <c r="B87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>248</v>
+      </c>
+      <c r="B88" t="s">
+        <v>195</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>249</v>
+      </c>
+      <c r="B89" t="s">
+        <v>274</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>250</v>
+      </c>
+      <c r="B90" t="s">
+        <v>276</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>251</v>
+      </c>
+      <c r="B91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>252</v>
+      </c>
+      <c r="B92" t="s">
+        <v>202</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>253</v>
+      </c>
+      <c r="B93" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>254</v>
+      </c>
+      <c r="B94" t="s">
+        <v>204</v>
+      </c>
+      <c r="C94" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>255</v>
+      </c>
+      <c r="B95" t="s">
+        <v>257</v>
+      </c>
+      <c r="C95" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>256</v>
+      </c>
+      <c r="B96" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>259</v>
+      </c>
+      <c r="B97" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>265</v>
+      </c>
+      <c r="B98" t="s">
+        <v>213</v>
+      </c>
+      <c r="C98" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>264</v>
+      </c>
+      <c r="B99" t="s">
+        <v>212</v>
+      </c>
+      <c r="C99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>260</v>
+      </c>
+      <c r="B100" t="s">
+        <v>266</v>
+      </c>
+      <c r="C100" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>261</v>
+      </c>
+      <c r="B101" t="s">
+        <v>270</v>
+      </c>
+      <c r="C101" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>262</v>
+      </c>
+      <c r="B102" t="s">
+        <v>268</v>
+      </c>
+      <c r="C102" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>263</v>
+      </c>
+      <c r="B103" t="s">
+        <v>272</v>
+      </c>
+      <c r="C103" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update translation default file
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="311">
   <si>
     <t>de_DE</t>
   </si>
@@ -934,6 +934,24 @@
   </si>
   <si>
     <t>The device wipe request has been successfully registered.</t>
+  </si>
+  <si>
+    <t>get_all_certification_courses_failed</t>
+  </si>
+  <si>
+    <t>get_certification_courses_by_ca_failed</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al recuperar el listado completo de cursos.</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al recuperar el listado de cursos de la CA.</t>
+  </si>
+  <si>
+    <t>An error occurred when retrieving the complete list of courses.</t>
+  </si>
+  <si>
+    <t>An error occurred while retrieving the list of courses from the CA.</t>
   </si>
 </sst>
 </file>
@@ -1342,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2592,6 +2610,28 @@
         <v>304</v>
       </c>
     </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>305</v>
+      </c>
+      <c r="B113" t="s">
+        <v>307</v>
+      </c>
+      <c r="C113" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>306</v>
+      </c>
+      <c r="B114" t="s">
+        <v>308</v>
+      </c>
+      <c r="C114" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[AUTHENTICATION] Implement User login register.
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="320">
   <si>
     <t>de_DE</t>
   </si>
@@ -952,6 +952,33 @@
   </si>
   <si>
     <t>An error occurred while retrieving the list of courses from the CA.</t>
+  </si>
+  <si>
+    <t>login_history_deleted</t>
+  </si>
+  <si>
+    <t>El historial de inicio de sesión fue eliminado con éxito</t>
+  </si>
+  <si>
+    <t>Login history deleted successfully</t>
+  </si>
+  <si>
+    <t>delete_loging_history_failed</t>
+  </si>
+  <si>
+    <t>Ocurrio un error al eliminar el historial de inicio de sesión fue eliminado con éxito</t>
+  </si>
+  <si>
+    <t>An error occurred while deleting the login history was deleted successfully</t>
+  </si>
+  <si>
+    <t>get_loging_history_failed</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al recuperar el historial de inicio de sesión</t>
+  </si>
+  <si>
+    <t>An error occurred while retrieving login history</t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2632,6 +2659,39 @@
         <v>310</v>
       </c>
     </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>311</v>
+      </c>
+      <c r="B115" t="s">
+        <v>312</v>
+      </c>
+      <c r="C115" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>314</v>
+      </c>
+      <c r="B116" t="s">
+        <v>315</v>
+      </c>
+      <c r="C116" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>317</v>
+      </c>
+      <c r="B117" t="s">
+        <v>318</v>
+      </c>
+      <c r="C117" t="s">
+        <v>319</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[AUTH] Implement Social authentication methods
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="332">
   <si>
     <t>de_DE</t>
   </si>
@@ -979,6 +979,42 @@
   </si>
   <si>
     <t>An error occurred while retrieving login history</t>
+  </si>
+  <si>
+    <t>provider_access_token_not_null</t>
+  </si>
+  <si>
+    <t>provider_type_invalid</t>
+  </si>
+  <si>
+    <t>sign_in_external_provider_failed</t>
+  </si>
+  <si>
+    <t>sign_up_external_provider_failed</t>
+  </si>
+  <si>
+    <t>Debes proporcionar un token de proveedor válido</t>
+  </si>
+  <si>
+    <t>You must provide a valid provider token</t>
+  </si>
+  <si>
+    <t>El tipo de proveedor especificado no es válido</t>
+  </si>
+  <si>
+    <t>The specified provider type is not valid</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al completar el inicio sesión a través del proovedor externo</t>
+  </si>
+  <si>
+    <t>An error occurred while completing the login through the external provider</t>
+  </si>
+  <si>
+    <t>Ocurrió un error al completar el registro a través del proovedor externo</t>
+  </si>
+  <si>
+    <t>An error occurred while completing the registration through the external provider</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2692,6 +2728,50 @@
         <v>319</v>
       </c>
     </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>320</v>
+      </c>
+      <c r="B118" t="s">
+        <v>324</v>
+      </c>
+      <c r="C118" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>321</v>
+      </c>
+      <c r="B119" t="s">
+        <v>326</v>
+      </c>
+      <c r="C119" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>322</v>
+      </c>
+      <c r="B120" t="s">
+        <v>328</v>
+      </c>
+      <c r="C120" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>323</v>
+      </c>
+      <c r="B121" t="s">
+        <v>330</v>
+      </c>
+      <c r="C121" t="s">
+        <v>331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>